<commit_message>
Cap nhat tối ưu hóa tốc độ
</commit_message>
<xml_diff>
--- a/All data.xlsx
+++ b/All data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6019702-3EAD-4A76-B49C-5734A3EEE0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="1875" yWindow="2820" windowWidth="14355" windowHeight="12060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XauUsd" sheetId="1" r:id="rId1"/>
@@ -12,10 +13,18 @@
     <sheet name="UsdChf" sheetId="3" r:id="rId3"/>
     <sheet name="UsdCad" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -42,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D1" sqref="D1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,30 +394,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>349</v>
+        <v>245</v>
       </c>
       <c r="B2">
-        <v>349</v>
+        <v>245</v>
       </c>
       <c r="D2" s="1">
-        <v>349</v>
+        <v>245</v>
       </c>
       <c r="E2">
-        <v>349</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2540.75</v>
+        <v>365.05</v>
       </c>
       <c r="B3">
-        <v>526</v>
+        <v>185.5</v>
       </c>
       <c r="D3" s="1">
-        <v>2540.75</v>
+        <v>365.05</v>
       </c>
       <c r="E3">
-        <v>526</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -427,30 +436,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>45.21</v>
+        <v>61.51</v>
       </c>
       <c r="B5">
-        <v>46.95</v>
+        <v>64.27</v>
       </c>
       <c r="D5">
-        <v>45.21</v>
+        <v>61.51</v>
       </c>
       <c r="E5">
-        <v>46.95</v>
+        <v>64.27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>43.25</v>
+        <v>54.41</v>
       </c>
       <c r="B6">
-        <v>52.69</v>
+        <v>51.29</v>
       </c>
       <c r="D6">
-        <v>43.25</v>
+        <v>54.41</v>
       </c>
       <c r="E6">
-        <v>52.69</v>
+        <v>51.29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,7 +497,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>E3-B3</f>
+        <f>B3-E3</f>
         <v>0</v>
       </c>
       <c r="B12" t="s">
@@ -498,11 +507,11 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A2-A3</f>
-        <v>-2191.75</v>
+        <v>-120.05000000000001</v>
       </c>
       <c r="B14">
         <f>B2-B3</f>
-        <v>-177</v>
+        <v>59.5</v>
       </c>
     </row>
   </sheetData>
@@ -511,11 +520,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D1" sqref="D1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,30 +545,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="D2">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1513.65</v>
+        <v>825.4</v>
       </c>
       <c r="B3">
-        <v>371.6</v>
+        <v>283.25</v>
       </c>
       <c r="D3">
-        <v>1513.65</v>
+        <v>825.4</v>
       </c>
       <c r="E3">
-        <v>371.6</v>
+        <v>283.25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -578,30 +587,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>55.8</v>
+        <v>51.84</v>
       </c>
       <c r="B5">
-        <v>48.04</v>
+        <v>52.23</v>
       </c>
       <c r="D5">
-        <v>55.8</v>
+        <v>51.84</v>
       </c>
       <c r="E5">
-        <v>48.04</v>
+        <v>52.23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>60.18</v>
+        <v>48.32</v>
       </c>
       <c r="B6">
-        <v>48.43</v>
+        <v>57.31</v>
       </c>
       <c r="D6">
-        <v>60.18</v>
+        <v>48.32</v>
       </c>
       <c r="E6">
-        <v>48.43</v>
+        <v>57.31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -639,7 +648,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>E3-B3</f>
+        <f>B3-E3</f>
         <v>0</v>
       </c>
       <c r="B12" t="s">
@@ -649,11 +658,11 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A2-A3</f>
-        <v>-1286.6500000000001</v>
+        <v>-632.4</v>
       </c>
       <c r="B14">
         <f>B2-B3</f>
-        <v>-371.6</v>
+        <v>-90.25</v>
       </c>
     </row>
   </sheetData>
@@ -662,11 +671,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,30 +696,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>246</v>
+        <v>105</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="D2">
-        <v>246</v>
+        <v>105</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1514.6</v>
+        <v>378.4</v>
       </c>
       <c r="B3">
-        <v>371.65</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="D3">
-        <v>1514.6</v>
+        <v>378.4</v>
       </c>
       <c r="E3">
-        <v>371.65</v>
+        <v>142.30000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,30 +738,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>56.16</v>
+        <v>41.93</v>
       </c>
       <c r="B5">
-        <v>48.24</v>
+        <v>45.5</v>
       </c>
       <c r="D5">
-        <v>56.16</v>
+        <v>41.93</v>
       </c>
       <c r="E5">
-        <v>48.24</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>60.2</v>
+        <v>42.4</v>
       </c>
       <c r="B6">
-        <v>48.44</v>
+        <v>47.83</v>
       </c>
       <c r="D6">
-        <v>60.2</v>
+        <v>42.4</v>
       </c>
       <c r="E6">
-        <v>48.44</v>
+        <v>47.83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,7 +799,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>E3-B3</f>
+        <f>B3-E3</f>
         <v>0</v>
       </c>
       <c r="B12" t="s">
@@ -800,11 +809,11 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A2-A3</f>
-        <v>-1268.5999999999999</v>
+        <v>-273.39999999999998</v>
       </c>
       <c r="B14">
         <f>B2-B3</f>
-        <v>-370.65</v>
+        <v>-37.300000000000011</v>
       </c>
     </row>
   </sheetData>
@@ -813,11 +822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,30 +847,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>429</v>
+        <v>250</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>250</v>
       </c>
       <c r="D2">
-        <v>429</v>
+        <v>250</v>
       </c>
       <c r="E2">
-        <v>9</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2092.5</v>
+        <v>615.79999999999995</v>
       </c>
       <c r="B3">
-        <v>550.65</v>
+        <v>269.05</v>
       </c>
       <c r="D3">
-        <v>2092.5</v>
+        <v>615.79999999999995</v>
       </c>
       <c r="E3">
-        <v>550.65</v>
+        <v>269.05</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -880,30 +889,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>50.57</v>
+        <v>51.64</v>
       </c>
       <c r="B5">
-        <v>52.82</v>
+        <v>51.71</v>
       </c>
       <c r="D5">
-        <v>50.57</v>
+        <v>51.64</v>
       </c>
       <c r="E5">
-        <v>52.82</v>
+        <v>51.71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>51.82</v>
+        <v>48.18</v>
       </c>
       <c r="B6">
-        <v>44.62</v>
+        <v>60.23</v>
       </c>
       <c r="D6">
-        <v>51.82</v>
+        <v>48.18</v>
       </c>
       <c r="E6">
-        <v>44.62</v>
+        <v>60.23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -941,7 +950,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>E3-B3</f>
+        <f>B3-E3</f>
         <v>0</v>
       </c>
       <c r="B12" t="s">
@@ -951,11 +960,11 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>A2-A3</f>
-        <v>-1663.5</v>
+        <v>-365.79999999999995</v>
       </c>
       <c r="B14">
         <f>B2-B3</f>
-        <v>-541.65</v>
+        <v>-19.050000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cap nhat lan N
</commit_message>
<xml_diff>
--- a/All data.xlsx
+++ b/All data.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFD9688-E4EC-40A7-9ED9-4A4E65D0C03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973D9F7C-9ED4-4930-901A-F50609CE2EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="1950" windowWidth="14355" windowHeight="12060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11895" yWindow="1950" windowWidth="14355" windowHeight="12060" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4H" sheetId="5" r:id="rId1"/>
     <sheet name="1H" sheetId="6" r:id="rId2"/>
     <sheet name="15m" sheetId="9" r:id="rId3"/>
     <sheet name="5m" sheetId="10" r:id="rId4"/>
+    <sheet name="4H Eur" sheetId="11" r:id="rId5"/>
+    <sheet name="1H Eur" sheetId="12" r:id="rId6"/>
+    <sheet name="15m Eur" sheetId="13" r:id="rId7"/>
+    <sheet name="5m Eur" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
   <si>
     <t>Rsi</t>
   </si>
@@ -51,22 +55,43 @@
     <t>khoi luong</t>
   </si>
   <si>
-    <t>+0.190 (+0.01%)</t>
-  </si>
-  <si>
-    <t>1.025K</t>
-  </si>
-  <si>
-    <t>+0.250 (+0.01%)</t>
-  </si>
-  <si>
-    <t>+0.570 (+0.03%)</t>
+    <t>−0.025 (−0.00%)</t>
+  </si>
+  <si>
+    <t>2.182K</t>
+  </si>
+  <si>
+    <t>+0.00092 (+0.09%)</t>
+  </si>
+  <si>
+    <t>5.642K</t>
+  </si>
+  <si>
+    <t>−0.810 (−0.05%)</t>
+  </si>
+  <si>
+    <t>−0.760 (−0.04%)</t>
+  </si>
+  <si>
+    <t>−0.430 (−0.03%)</t>
+  </si>
+  <si>
+    <t>−0.00050 (−0.05%)</t>
+  </si>
+  <si>
+    <t>−0.00056 (−0.06%)</t>
+  </si>
+  <si>
+    <t>+0.00043 (+0.04%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,60 +422,60 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2">
-        <v>1669.7529999999999</v>
+        <v>1694.37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1674.115</v>
+        <v>1713.2850000000001</v>
       </c>
       <c r="C3">
-        <v>1681.261</v>
+        <v>1742.617</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1674.6849999999999</v>
+        <v>1713.78</v>
       </c>
       <c r="C4">
-        <v>1658.2449999999999</v>
+        <v>1646.124</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1673.15</v>
+        <v>1712.4749999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1674.3050000000001</v>
+        <v>1712.4749999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1674.3050000000001</v>
+        <v>1712.4749999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+      <c r="A10">
+        <v>603</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>C3-A6</f>
-        <v>6.9559999999999036</v>
+        <v>30.142000000000053</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A6-C4</f>
-        <v>16.060000000000173</v>
+        <v>66.350999999999885</v>
       </c>
     </row>
   </sheetData>
@@ -477,60 +503,60 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2">
-        <v>1667.4</v>
+        <v>1718.924</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1674.115</v>
+        <v>1713.2850000000001</v>
       </c>
       <c r="C3">
-        <v>1680.1179999999999</v>
+        <v>1731.1690000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1674.6849999999999</v>
+        <v>1713.78</v>
       </c>
       <c r="C4">
-        <v>1654.681</v>
+        <v>1706.6790000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1673.15</v>
+        <v>1712.4749999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1674.3050000000001</v>
+        <v>1712.5250000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1674.3050000000001</v>
+        <v>1712.5250000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+      <c r="A10">
+        <v>603</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>C3-A6</f>
-        <v>5.8129999999998745</v>
+        <v>18.644000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A6-C4</f>
-        <v>19.624000000000024</v>
+        <v>5.8460000000000036</v>
       </c>
     </row>
   </sheetData>
@@ -540,6 +566,587 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDBB260-1F1F-4C65-8F5B-91398819A9F3}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1710.577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1711.425</v>
+      </c>
+      <c r="C3">
+        <v>1717.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1713.335</v>
+      </c>
+      <c r="C4">
+        <v>1703.8330000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1710.155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1711.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1711.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>C3-A6</f>
+        <v>5.9199999999998454</v>
+      </c>
+      <c r="C12">
+        <f>A6-C2</f>
+        <v>0.82300000000009277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A6-C4</f>
+        <v>7.5670000000000073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2182</v>
+      </c>
+      <c r="C16">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1703.6</v>
+      </c>
+      <c r="C17">
+        <v>1703.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>A16-A17</f>
+        <v>478.40000000000009</v>
+      </c>
+      <c r="C19">
+        <f>A17-C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>47.69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>38.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9F0CDB-5BD8-4956-8E77-15F4CC02BC66}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1709.097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1713.2850000000001</v>
+      </c>
+      <c r="C3">
+        <v>1714.701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1713.78</v>
+      </c>
+      <c r="C4">
+        <v>1703.4929999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1712.4749999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1712.855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1712.855</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>C3-A6</f>
+        <v>1.8460000000000036</v>
+      </c>
+      <c r="C12">
+        <f>A6-C2</f>
+        <v>3.7580000000000382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A6-C4</f>
+        <v>9.36200000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>655</v>
+      </c>
+      <c r="C16">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>823.6</v>
+      </c>
+      <c r="C17">
+        <v>823.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>A16-A17</f>
+        <v>-168.60000000000002</v>
+      </c>
+      <c r="C19">
+        <f>A17-C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>37.369999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3599490-A5E1-402D-A313-DD65F06837E7}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>0.98634999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.99117999999999995</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.00153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.99143000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.97116000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.99068000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.99068000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.99068000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>C3-A6</f>
+        <v>1.0850000000000026E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f>A6-C4</f>
+        <v>1.9519999999999982E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9A63B8-1F60-45C9-961D-BAC43991AAA2}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0.99626000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.99053999999999998</v>
+      </c>
+      <c r="C3">
+        <v>1.0014400000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.99231999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.99107000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.98985999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.99146000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.99146000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>C3-A6</f>
+        <v>9.9800000000000999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f>A6-C4</f>
+        <v>3.9000000000000146E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862A5F52-1CCA-46FC-9375-2CD6F8B32CB2}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0.99226000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.99117999999999995</v>
+      </c>
+      <c r="C3">
+        <v>0.99487999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.99143000000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.98965000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.99061999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.99061999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.99061999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>C3-A6</f>
+        <v>4.2600000000000415E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A6-C4</f>
+        <v>9.6999999999991537E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>641</v>
+      </c>
+      <c r="C16">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1587</v>
+      </c>
+      <c r="C17">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>35.729999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>34.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9E79D6-2413-4710-AB06-F8BEE68CD70D}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -557,65 +1164,61 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>1674.5419999999999</v>
+      <c r="C2" s="1">
+        <v>0.99761</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1674.115</v>
-      </c>
-      <c r="C3">
-        <v>1682.482</v>
+      <c r="A3" s="1">
+        <v>0.99658000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.99870000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1674.6849999999999</v>
-      </c>
-      <c r="C4">
-        <v>1666.6020000000001</v>
+      <c r="A4" s="1">
+        <v>0.99731000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.99653000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1673.15</v>
+      <c r="A5" s="1">
+        <v>0.99643999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1674.365</v>
+      <c r="A6" s="1">
+        <v>0.99700999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1674.365</v>
+      <c r="A7" s="1">
+        <v>0.99700999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
+      <c r="A10">
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <f>C3-A6</f>
-        <v>8.1169999999999618</v>
-      </c>
-      <c r="C12">
-        <f>A6-C2</f>
-        <v>-0.17699999999990723</v>
+        <v>1.6900000000000803E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <f>A6-C4</f>
-        <v>7.76299999999992</v>
+        <v>4.7999999999992493E-4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,28 +1231,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1025</v>
+        <v>569</v>
       </c>
       <c r="C16">
-        <v>1025</v>
+        <v>569</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2845.05</v>
+        <v>527.29999999999995</v>
       </c>
       <c r="C17">
-        <v>2845.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>A16-A17</f>
-        <v>-1820.0500000000002</v>
-      </c>
-      <c r="C19">
-        <f>A17-C17</f>
-        <v>0</v>
+        <v>527.29999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,12 +1252,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>55.07</v>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>51.72</v>
+        <v>44.95</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,149 +1272,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9F0CDB-5BD8-4956-8E77-15F4CC02BC66}">
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>1672.6479999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1673.82</v>
-      </c>
-      <c r="C3">
-        <v>1675.115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1674.43</v>
-      </c>
-      <c r="C4">
-        <v>1670.182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1673.7149999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1674.39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1674.39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>C3-A6</f>
-        <v>0.72499999999990905</v>
-      </c>
-      <c r="C12">
-        <f>A6-C2</f>
-        <v>1.7420000000001892</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>A6-C4</f>
-        <v>4.2080000000000837</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>123</v>
-      </c>
-      <c r="C16">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>499.25</v>
-      </c>
-      <c r="C17">
-        <v>309.64999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>A16-A17</f>
-        <v>-376.25</v>
-      </c>
-      <c r="C19">
-        <f>A17-C17</f>
-        <v>189.60000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>57.17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>